<commit_message>
atualização da planilha de riscos
</commit_message>
<xml_diff>
--- a/Apresentação segunda sprint/PRODUCT SPRINT RISCOS.xlsx
+++ b/Apresentação segunda sprint/PRODUCT SPRINT RISCOS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Apresentação segunda sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="163">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -449,12 +449,6 @@
     <t>Atraso na entrega das atividades (sprint)</t>
   </si>
   <si>
-    <t>Médio (2)</t>
-  </si>
-  <si>
-    <t>Provável (2)</t>
-  </si>
-  <si>
     <t>Eliminar</t>
   </si>
   <si>
@@ -464,21 +458,9 @@
     <t>Falta de conhecimento</t>
   </si>
   <si>
-    <t>Pouco (1)</t>
-  </si>
-  <si>
-    <t>Baixo(1)</t>
-  </si>
-  <si>
-    <t>Nivelar o máximo possivél para não haver chances do conhecimento ficar com alguns ou com um integrante do grupo só.</t>
-  </si>
-  <si>
     <t>Falta de internet durante aula.</t>
   </si>
   <si>
-    <t>Alto (3)</t>
-  </si>
-  <si>
     <t>Aceitar</t>
   </si>
   <si>
@@ -494,19 +476,40 @@
     <t>Falta de membro em uma aula.</t>
   </si>
   <si>
-    <t>Iremos passar a informação que nos foi apresentada na aula para o membro que faltou.</t>
-  </si>
-  <si>
     <t>Desconforto de algum membro</t>
   </si>
   <si>
     <t>RISCOS</t>
   </si>
   <si>
-    <t>Caso o dano não afete o desempenho do sensor no Arduino podemos continuar a utiliza-lo.</t>
-  </si>
-  <si>
     <t>Tentando deixar o ambiente de projeto o mais agradável possivel para os integrantes do grupo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alto </t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provável </t>
+  </si>
+  <si>
+    <t>Pouco provável</t>
+  </si>
+  <si>
+    <t>Muito provável</t>
+  </si>
+  <si>
+    <t>Caso o dano não afete o desempenho dos sensores ou do Arduino podemos continuar    a utiliza-los.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iremos passar a informação que nos foi apresentada em aula para o membro que    não pode comparecer. </t>
+  </si>
+  <si>
+    <t>Nivelar o máximo possivél para não haver chances do conhecimento ficar com alguns    ou com um integrante do grupo só.</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -627,6 +630,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1329,7 +1350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1416,89 +1437,113 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1508,32 +1553,20 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1830,13 +1863,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="34"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="49"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -1906,7 +1939,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
         <v>27</v>
       </c>
@@ -2955,16 +2988,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
     </row>
     <row r="3" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -2993,16 +3026,16 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="65" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="15" t="s">
@@ -3019,41 +3052,41 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="46"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="37" t="s">
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="50">
         <v>43559</v>
       </c>
-      <c r="I5" s="50" t="s">
+      <c r="I5" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="46"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="44"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="54"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="37" t="s">
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="52" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="24" t="s">
@@ -3070,10 +3103,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="24" t="s">
         <v>44</v>
       </c>
@@ -3088,70 +3121,70 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="46"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="37" t="s">
+      <c r="B9" s="59"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="50">
         <v>43559</v>
       </c>
-      <c r="I9" s="50" t="s">
+      <c r="I9" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="46"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="44"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="54"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="46"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
-      <c r="F11" s="37" t="s">
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="38">
+      <c r="H11" s="50">
         <v>43559</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="46"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="44"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="54"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B13" s="46"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
       <c r="F13" s="24" t="s">
         <v>52</v>
       </c>
@@ -3166,10 +3199,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="24" t="s">
         <v>54</v>
       </c>
@@ -3194,104 +3227,104 @@
       <c r="I15" s="31"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="H16" s="38">
+      <c r="H16" s="50">
         <v>43563</v>
       </c>
-      <c r="I16" s="50" t="s">
+      <c r="I16" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="46"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="44"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="54"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="46"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="37" t="s">
+      <c r="B18" s="59"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H18" s="50">
         <v>43563</v>
       </c>
-      <c r="I18" s="50" t="s">
+      <c r="I18" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="46"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="44"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="54"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="46"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="37" t="s">
+      <c r="B20" s="59"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="57" t="s">
         <v>64</v>
       </c>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="H20" s="38">
+      <c r="H20" s="50">
         <v>43572</v>
       </c>
-      <c r="I20" s="50" t="s">
+      <c r="I20" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="46"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="44"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="46"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="37" t="s">
+      <c r="B22" s="59"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="52" t="s">
         <v>67</v>
       </c>
       <c r="F22" s="24" t="s">
@@ -3309,10 +3342,10 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="24" t="s">
         <v>70</v>
       </c>
@@ -3327,12 +3360,12 @@
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="46"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="37" t="s">
+      <c r="B24" s="59"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="E24" s="52" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="24" t="s">
@@ -3349,10 +3382,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="46"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
       <c r="F25" s="24" t="s">
         <v>76</v>
       </c>
@@ -3367,10 +3400,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="24" t="s">
         <v>78</v>
       </c>
@@ -3395,249 +3428,249 @@
       <c r="I27" s="31"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="F28" s="37" t="s">
+      <c r="F28" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="G28" s="52" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="38">
+      <c r="H28" s="50">
         <v>43565</v>
       </c>
-      <c r="I28" s="50" t="s">
+      <c r="I28" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="46"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="44"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="54"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="46"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="37" t="s">
+      <c r="B30" s="59"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="H30" s="38">
+      <c r="H30" s="50">
         <v>43565</v>
       </c>
-      <c r="I30" s="50" t="s">
+      <c r="I30" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="46"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="44"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="54"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="46"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
-      <c r="E32" s="49"/>
-      <c r="F32" s="37" t="s">
+      <c r="B32" s="59"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57" t="s">
         <v>88</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H32" s="50">
         <v>43565</v>
       </c>
-      <c r="I32" s="50" t="s">
+      <c r="I32" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="46"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="44"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="54"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="46"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="37" t="s">
+      <c r="B34" s="59"/>
+      <c r="C34" s="56"/>
+      <c r="D34" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="37" t="s">
+      <c r="F34" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="G34" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="H34" s="38">
+      <c r="H34" s="50">
         <v>43565</v>
       </c>
-      <c r="I34" s="50" t="s">
+      <c r="I34" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
-      <c r="B35" s="46"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="44"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="54"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="46"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="37" t="s">
+      <c r="B36" s="59"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="H36" s="38">
+      <c r="H36" s="50">
         <v>43565</v>
       </c>
-      <c r="I36" s="50" t="s">
+      <c r="I36" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="46"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="44"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="54"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="46"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="37" t="s">
+      <c r="B38" s="59"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="F38" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="H38" s="38">
+      <c r="H38" s="50">
         <v>43565</v>
       </c>
-      <c r="I38" s="50" t="s">
+      <c r="I38" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="46"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="44"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="56"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="54"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="46"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="37" t="s">
+      <c r="B40" s="59"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="H40" s="38">
+      <c r="H40" s="50">
         <v>43565</v>
       </c>
-      <c r="I40" s="50" t="s">
+      <c r="I40" s="53" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="46"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="44"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="56"/>
+      <c r="D41" s="56"/>
+      <c r="E41" s="56"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="51"/>
+      <c r="H41" s="51"/>
+      <c r="I41" s="54"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="46"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="37" t="s">
+      <c r="B42" s="59"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G42" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="H42" s="38">
+      <c r="H42" s="50">
         <v>43579</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="56"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="44"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="54"/>
     </row>
     <row r="44" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="29"/>
@@ -3651,89 +3684,89 @@
     </row>
     <row r="45" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
-      <c r="B45" s="55" t="s">
+      <c r="B45" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G45" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="H45" s="38">
+      <c r="H45" s="50">
         <v>43579</v>
       </c>
-      <c r="I45" s="40" t="s">
+      <c r="I45" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
-      <c r="B46" s="46"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="I46" s="52"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="69"/>
     </row>
     <row r="47" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="46"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="44"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="51"/>
+      <c r="H47" s="51"/>
+      <c r="I47" s="54"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="46"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="37" t="s">
+      <c r="B48" s="59"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="G48" s="35" t="s">
+      <c r="G48" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="38">
+      <c r="H48" s="50">
         <v>43579</v>
       </c>
-      <c r="I48" s="40" t="s">
+      <c r="I48" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="46"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="I49" s="52"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="69"/>
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="56"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="44"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="51"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="51"/>
+      <c r="H50" s="51"/>
+      <c r="I50" s="54"/>
     </row>
     <row r="51" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="29"/>
@@ -3746,241 +3779,241 @@
       <c r="I51" s="31"/>
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="45" t="s">
+      <c r="B52" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="C52" s="48" t="s">
+      <c r="C52" s="72" t="s">
         <v>113</v>
       </c>
-      <c r="D52" s="42" t="s">
+      <c r="D52" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="48" t="s">
+      <c r="E52" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="F52" s="42" t="s">
+      <c r="F52" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="G52" s="48" t="s">
+      <c r="G52" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="H52" s="43">
+      <c r="H52" s="75">
         <v>43570</v>
       </c>
-      <c r="I52" s="51" t="s">
+      <c r="I52" s="67" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="46"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
-      <c r="E53" s="49"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="44"/>
+      <c r="B53" s="59"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="51"/>
+      <c r="G53" s="51"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="54"/>
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="46"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="49"/>
-      <c r="F54" s="37" t="s">
+      <c r="B54" s="59"/>
+      <c r="C54" s="56"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="57" t="s">
         <v>118</v>
       </c>
-      <c r="G54" s="35" t="s">
+      <c r="G54" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="H54" s="38">
+      <c r="H54" s="50">
         <v>43570</v>
       </c>
-      <c r="I54" s="40" t="s">
+      <c r="I54" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
-      <c r="E55" s="49"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="44"/>
+      <c r="B55" s="59"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="54"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="46"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
-      <c r="E56" s="49"/>
-      <c r="F56" s="37" t="s">
+      <c r="B56" s="59"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="H56" s="38">
+      <c r="H56" s="50">
         <v>43570</v>
       </c>
-      <c r="I56" s="40" t="s">
+      <c r="I56" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="46"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="49"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="44"/>
+      <c r="B57" s="59"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
+      <c r="E57" s="56"/>
+      <c r="F57" s="51"/>
+      <c r="G57" s="51"/>
+      <c r="H57" s="51"/>
+      <c r="I57" s="54"/>
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="46"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
-      <c r="E58" s="49"/>
-      <c r="F58" s="37" t="s">
+      <c r="B58" s="59"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="56"/>
+      <c r="E58" s="56"/>
+      <c r="F58" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="G58" s="35" t="s">
+      <c r="G58" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="H58" s="38">
+      <c r="H58" s="50">
         <v>43579</v>
       </c>
-      <c r="I58" s="40" t="s">
+      <c r="I58" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="46"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="44"/>
+      <c r="B59" s="59"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+      <c r="H59" s="51"/>
+      <c r="I59" s="54"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="46"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="37" t="s">
+      <c r="B60" s="59"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="E60" s="35" t="s">
+      <c r="E60" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="F60" s="37" t="s">
+      <c r="F60" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="G60" s="35" t="s">
+      <c r="G60" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="H60" s="38">
+      <c r="H60" s="50">
         <v>43570</v>
       </c>
-      <c r="I60" s="40" t="s">
+      <c r="I60" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="46"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="44"/>
+      <c r="B61" s="59"/>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="51"/>
+      <c r="H61" s="51"/>
+      <c r="I61" s="54"/>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="46"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="37" t="s">
+      <c r="B62" s="59"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="G62" s="35" t="s">
+      <c r="G62" s="52" t="s">
         <v>129</v>
       </c>
-      <c r="H62" s="38">
+      <c r="H62" s="50">
         <v>43570</v>
       </c>
-      <c r="I62" s="40" t="s">
+      <c r="I62" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="46"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="44"/>
+      <c r="B63" s="59"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="51"/>
+      <c r="G63" s="51"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="54"/>
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="46"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
-      <c r="E64" s="49"/>
-      <c r="F64" s="37" t="s">
+      <c r="B64" s="59"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="G64" s="35" t="s">
+      <c r="G64" s="52" t="s">
         <v>131</v>
       </c>
-      <c r="H64" s="38">
+      <c r="H64" s="50">
         <v>43579</v>
       </c>
-      <c r="I64" s="40" t="s">
+      <c r="I64" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="65" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="46"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
-      <c r="E65" s="49"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="36"/>
-      <c r="H65" s="36"/>
-      <c r="I65" s="44"/>
+      <c r="B65" s="59"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="51"/>
+      <c r="G65" s="51"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="54"/>
     </row>
     <row r="66" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="46"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
-      <c r="E66" s="49"/>
-      <c r="F66" s="37" t="s">
+      <c r="B66" s="59"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="G66" s="35" t="s">
+      <c r="G66" s="52" t="s">
         <v>133</v>
       </c>
-      <c r="H66" s="38">
+      <c r="H66" s="50">
         <v>43579</v>
       </c>
-      <c r="I66" s="40" t="s">
+      <c r="I66" s="68" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="67" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="47"/>
-      <c r="C67" s="39"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="39"/>
-      <c r="I67" s="41"/>
+      <c r="B67" s="71"/>
+      <c r="C67" s="73"/>
+      <c r="D67" s="73"/>
+      <c r="E67" s="73"/>
+      <c r="F67" s="73"/>
+      <c r="G67" s="73"/>
+      <c r="H67" s="73"/>
+      <c r="I67" s="76"/>
     </row>
     <row r="68" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4917,43 +4950,76 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="133">
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="H36:H37"/>
-    <mergeCell ref="I36:I37"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="I56:I57"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="H56:H57"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="B52:B67"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="G45:G47"/>
+    <mergeCell ref="G48:G50"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="C52:C67"/>
+    <mergeCell ref="E52:E59"/>
+    <mergeCell ref="E60:E67"/>
+    <mergeCell ref="D52:D59"/>
+    <mergeCell ref="D60:D67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="I52:I53"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="H45:H47"/>
+    <mergeCell ref="H42:H43"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="I48:I50"/>
+    <mergeCell ref="I42:I43"/>
+    <mergeCell ref="H52:H53"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="F34:F35"/>
     <mergeCell ref="D34:D37"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E34:E37"/>
@@ -4978,78 +5044,45 @@
     <mergeCell ref="E24:E26"/>
     <mergeCell ref="D28:D33"/>
     <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="E16:E21"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
     <mergeCell ref="E9:E14"/>
     <mergeCell ref="E4:E6"/>
-    <mergeCell ref="E28:E33"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="H38:H39"/>
-    <mergeCell ref="H40:H41"/>
-    <mergeCell ref="I52:I53"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="H45:H47"/>
-    <mergeCell ref="H42:H43"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="H48:H50"/>
-    <mergeCell ref="I48:I50"/>
-    <mergeCell ref="I42:I43"/>
-    <mergeCell ref="B52:B67"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="G48:G50"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="C52:C67"/>
-    <mergeCell ref="E52:E59"/>
-    <mergeCell ref="E60:E67"/>
-    <mergeCell ref="D52:D59"/>
-    <mergeCell ref="D60:D67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="H52:H53"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="I56:I57"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="H56:H57"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="I32:I33"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -5061,7 +5094,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5076,176 +5109,176 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="77" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="79"/>
+    </row>
+    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="38">
+        <v>1</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="80">
+        <v>3</v>
+      </c>
+      <c r="G4" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37"/>
+      <c r="B5" s="33">
+        <v>2</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F5" s="82">
+        <v>2</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="33">
+        <v>3</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="71"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="77" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="76" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="75" t="s">
-        <v>136</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="F3" s="75" t="s">
-        <v>138</v>
-      </c>
-      <c r="G3" s="75" t="s">
-        <v>139</v>
-      </c>
-      <c r="H3" s="78" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="72">
+      <c r="E6" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="81">
+        <v>3</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="33">
+        <v>4</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" s="83">
+        <v>2</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="33">
+        <v>5</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="83">
+        <v>2</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="35">
+        <v>6</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="84">
         <v>1</v>
       </c>
-      <c r="C4" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="D4" s="73" t="s">
+      <c r="G9" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="73" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="73">
-        <v>2</v>
-      </c>
-      <c r="G4" s="73" t="s">
-        <v>144</v>
-      </c>
-      <c r="H4" s="74" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
-      <c r="B5" s="64">
-        <v>2</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" s="63">
-        <v>1</v>
-      </c>
-      <c r="G5" s="62" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="64">
-        <v>3</v>
-      </c>
-      <c r="C6" s="62" t="s">
-        <v>150</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" s="62">
-        <v>3</v>
-      </c>
-      <c r="G6" s="62" t="s">
-        <v>152</v>
-      </c>
-      <c r="H6" s="65" t="s">
+      <c r="H9" s="46" t="s">
         <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="64">
-        <v>4</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>154</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="62" t="s">
-        <v>148</v>
-      </c>
-      <c r="F7" s="62">
-        <v>2</v>
-      </c>
-      <c r="G7" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="H7" s="79" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="64">
-        <v>5</v>
-      </c>
-      <c r="C8" s="62" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>151</v>
-      </c>
-      <c r="F8" s="62">
-        <v>2</v>
-      </c>
-      <c r="G8" s="62" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="65" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="66">
-        <v>6</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>158</v>
-      </c>
-      <c r="D9" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="67" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="67">
-        <v>1</v>
-      </c>
-      <c r="G9" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="H9" s="80" t="s">
-        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>